<commit_message>
add baseline data and check timeline
</commit_message>
<xml_diff>
--- a/ProjectManagement.xlsx
+++ b/ProjectManagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyhu\Desktop\w241experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB260AE-3713-4154-A17A-F08FBB2C333A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A7397-E7C8-4504-ACF2-7F5737C00280}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15380" xr2:uid="{E69ECB88-8EDB-4550-98F7-33033A131794}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15375" activeTab="1" xr2:uid="{E69ECB88-8EDB-4550-98F7-33033A131794}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>Treatment Units</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>all data done</t>
+  </si>
+  <si>
+    <t>flyer, post card</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -180,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,22 +589,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43A0EA7-A724-4684-B82D-3E3D4CECE36F}">
-  <dimension ref="C8:H17"/>
+  <dimension ref="A8:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
     <col min="6" max="7" width="24" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.1796875" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
@@ -611,7 +624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>43164</v>
       </c>
@@ -629,7 +642,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <f>D9</f>
         <v>43167</v>
@@ -653,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
         <f>Table1[[#This Row],[EndDate]]-6</f>
         <v>43168</v>
@@ -677,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="3:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="5">
         <f>C9</f>
         <v>43164</v>
@@ -701,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <f>Table1[[#This Row],[EndDate]]-3</f>
         <v>43171</v>
@@ -723,7 +736,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="3:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="6">
         <f>Table1[[#This Row],[EndDate]]</f>
         <v>43175</v>
@@ -747,7 +760,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="7">
+        <v>43182</v>
+      </c>
       <c r="C15" s="5">
         <f>Table1[[#This Row],[EndDate]]-13</f>
         <v>43182</v>
@@ -769,7 +788,13 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43202</v>
+      </c>
       <c r="C16" s="5">
         <f>Table1[[#This Row],[EndDate]]-13</f>
         <v>43196</v>
@@ -791,7 +816,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="6">
         <v>43210</v>
       </c>
@@ -824,29 +849,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FF779B-5065-45BC-870B-190C3F9998DC}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -860,7 +885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -869,13 +894,13 @@
       </c>
       <c r="C3" s="3">
         <f>B3*$B$1</f>
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -890,7 +915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -905,7 +930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -914,10 +939,10 @@
       </c>
       <c r="C6" s="3">
         <f>B6*$B$1</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -928,13 +953,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="4">
         <f>SUM(C3:C6)</f>
-        <v>338</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cost and combine design and report folders
</commit_message>
<xml_diff>
--- a/ProjectManagement.xlsx
+++ b/ProjectManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyhu\Desktop\w241experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A7397-E7C8-4504-ACF2-7F5737C00280}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09145329-4CF9-4F68-9167-769B40C47AC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15375" activeTab="1" xr2:uid="{E69ECB88-8EDB-4550-98F7-33033A131794}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>A4</t>
+  </si>
+  <si>
+    <t>12 inches * 7.5 inches, 100 copies, $150, a day, $20 for putting address</t>
+  </si>
+  <si>
+    <t>postcard</t>
+  </si>
+  <si>
+    <t>mailing label</t>
+  </si>
+  <si>
+    <t>Postcard</t>
   </si>
 </sst>
 </file>
@@ -180,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -188,11 +200,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -205,6 +232,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FF779B-5065-45BC-870B-190C3F9998DC}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +999,53 @@
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8">
+        <f>0.6*B16</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4">
+        <f>SUM(B17:B19)</f>
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>